<commit_message>
Intro BA: all examoles done before test
</commit_message>
<xml_diff>
--- a/Introduction_to_Business_Analytics/Examples/Lecture 11 - Linear Programming in Excel.xlsx
+++ b/Introduction_to_Business_Analytics/Examples/Lecture 11 - Linear Programming in Excel.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10916"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28025"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="2513" documentId="14_{2882EC59-6F6B-884B-9CA6-BCF321483F28}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C56E1EEE-020F-7F4F-BF78-F916914CCBB3}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E2DA783-2DA9-4C1C-89B3-1C8B51BF0C7F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5220" yWindow="500" windowWidth="42480" windowHeight="27860" tabRatio="828" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="828" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Portfolio Selection" sheetId="8" r:id="rId1"/>
@@ -89,6 +89,10 @@
     <definedName name="qpsolver_tol" localSheetId="2" hidden="1">0.05</definedName>
     <definedName name="qpsolver_tol" localSheetId="0" hidden="1">0.05</definedName>
     <definedName name="sencount" hidden="1">19</definedName>
+    <definedName name="solver_adj" localSheetId="1" hidden="1">'Blending Problem'!$B$16:$C$18</definedName>
+    <definedName name="solver_adj" localSheetId="2" hidden="1">'Marketing Research'!$B$13:$C$14</definedName>
+    <definedName name="solver_adj" localSheetId="3" hidden="1">'Media Selection'!$B$10:$D$11,'Media Selection'!$D$12</definedName>
+    <definedName name="solver_adj" localSheetId="0" hidden="1">'Portfolio Selection'!$B$26:$B$30</definedName>
     <definedName name="solver_cvg" localSheetId="1" hidden="1">0.0001</definedName>
     <definedName name="solver_cvg" localSheetId="2" hidden="1">0.0001</definedName>
     <definedName name="solver_cvg" localSheetId="3" hidden="1">0.0001</definedName>
@@ -97,10 +101,10 @@
     <definedName name="solver_drv" localSheetId="2" hidden="1">1</definedName>
     <definedName name="solver_drv" localSheetId="3" hidden="1">1</definedName>
     <definedName name="solver_drv" localSheetId="0" hidden="1">1</definedName>
-    <definedName name="solver_eng" localSheetId="1" hidden="1">1</definedName>
-    <definedName name="solver_eng" localSheetId="2" hidden="1">1</definedName>
+    <definedName name="solver_eng" localSheetId="1" hidden="1">2</definedName>
+    <definedName name="solver_eng" localSheetId="2" hidden="1">2</definedName>
     <definedName name="solver_eng" localSheetId="3" hidden="1">1</definedName>
-    <definedName name="solver_eng" localSheetId="0" hidden="1">1</definedName>
+    <definedName name="solver_eng" localSheetId="0" hidden="1">2</definedName>
     <definedName name="solver_est" localSheetId="1" hidden="1">1</definedName>
     <definedName name="solver_est" localSheetId="2" hidden="1">1</definedName>
     <definedName name="solver_est" localSheetId="3" hidden="1">1</definedName>
@@ -112,28 +116,43 @@
     <definedName name="solver_itr" localSheetId="2" hidden="1">2147483647</definedName>
     <definedName name="solver_itr" localSheetId="3" hidden="1">2147483647</definedName>
     <definedName name="solver_itr" localSheetId="0" hidden="1">2147483647</definedName>
-    <definedName name="solver_lhs1" localSheetId="1" hidden="1">'Blending Problem'!$G$18:$G$21</definedName>
-    <definedName name="solver_lhs1" localSheetId="2" hidden="1">'Marketing Research'!$B$13:$C$14</definedName>
-    <definedName name="solver_lhs1" localSheetId="3" hidden="1">'Media Selection'!$G$14:$G$16</definedName>
-    <definedName name="solver_lhs1" localSheetId="0" hidden="1">'Portfolio Selection'!$E$28:$E$30</definedName>
-    <definedName name="solver_lhs2" localSheetId="1" hidden="1">'Blending Problem'!$G$22</definedName>
-    <definedName name="solver_lhs2" localSheetId="2" hidden="1">'Marketing Research'!$H$14</definedName>
-    <definedName name="solver_lhs2" localSheetId="3" hidden="1">'Media Selection'!$G$17:$G$23</definedName>
-    <definedName name="solver_lhs2" localSheetId="0" hidden="1">'Portfolio Selection'!$E$31</definedName>
-    <definedName name="solver_lhs3" localSheetId="1" hidden="1">'Blending Problem'!$G$23</definedName>
-    <definedName name="solver_lhs3" localSheetId="2" hidden="1">'Marketing Research'!$H$15:$H$19</definedName>
-    <definedName name="solver_lhs3" localSheetId="3" hidden="1">'Media Selection'!$G$24:$G$26</definedName>
-    <definedName name="solver_lhs3" localSheetId="0" hidden="1">'Portfolio Selection'!$E$32</definedName>
-    <definedName name="solver_lhs4" localSheetId="1" hidden="1">'Blending Problem'!$G$24</definedName>
-    <definedName name="solver_lhs4" localSheetId="3" hidden="1">'Media Selection'!$G$27:$G$29</definedName>
+    <definedName name="solver_lhs1" localSheetId="1" hidden="1">'Blending Problem'!$G$18</definedName>
+    <definedName name="solver_lhs1" localSheetId="2" hidden="1">'Marketing Research'!$H$14</definedName>
+    <definedName name="solver_lhs1" localSheetId="3" hidden="1">'Media Selection'!$G$14</definedName>
+    <definedName name="solver_lhs1" localSheetId="0" hidden="1">'Portfolio Selection'!$E$28</definedName>
+    <definedName name="solver_lhs10" localSheetId="1" hidden="1">'Blending Problem'!$G$27</definedName>
+    <definedName name="solver_lhs10" localSheetId="3" hidden="1">'Media Selection'!$G$23</definedName>
+    <definedName name="solver_lhs11" localSheetId="3" hidden="1">'Media Selection'!$G$24</definedName>
+    <definedName name="solver_lhs12" localSheetId="3" hidden="1">'Media Selection'!$G$25</definedName>
+    <definedName name="solver_lhs13" localSheetId="3" hidden="1">'Media Selection'!$G$26</definedName>
+    <definedName name="solver_lhs14" localSheetId="3" hidden="1">'Media Selection'!$G$27</definedName>
+    <definedName name="solver_lhs15" localSheetId="3" hidden="1">'Media Selection'!$G$28</definedName>
+    <definedName name="solver_lhs16" localSheetId="3" hidden="1">'Media Selection'!$G$29</definedName>
+    <definedName name="solver_lhs2" localSheetId="1" hidden="1">'Blending Problem'!$G$19</definedName>
+    <definedName name="solver_lhs2" localSheetId="2" hidden="1">'Marketing Research'!$H$15</definedName>
+    <definedName name="solver_lhs2" localSheetId="3" hidden="1">'Media Selection'!$G$15</definedName>
+    <definedName name="solver_lhs2" localSheetId="0" hidden="1">'Portfolio Selection'!$E$29</definedName>
+    <definedName name="solver_lhs3" localSheetId="1" hidden="1">'Blending Problem'!$G$20</definedName>
+    <definedName name="solver_lhs3" localSheetId="2" hidden="1">'Marketing Research'!$H$16</definedName>
+    <definedName name="solver_lhs3" localSheetId="3" hidden="1">'Media Selection'!$G$16</definedName>
+    <definedName name="solver_lhs3" localSheetId="0" hidden="1">'Portfolio Selection'!$E$30</definedName>
+    <definedName name="solver_lhs4" localSheetId="1" hidden="1">'Blending Problem'!$G$21</definedName>
+    <definedName name="solver_lhs4" localSheetId="2" hidden="1">'Marketing Research'!$H$17</definedName>
+    <definedName name="solver_lhs4" localSheetId="3" hidden="1">'Media Selection'!$G$17</definedName>
     <definedName name="solver_lhs4" localSheetId="0" hidden="1">'Portfolio Selection'!$E$31</definedName>
-    <definedName name="solver_lhs5" localSheetId="1" hidden="1">'Blending Problem'!$G$25</definedName>
-    <definedName name="solver_lhs5" localSheetId="3" hidden="1">'Media Selection'!$G$24:$G$26</definedName>
+    <definedName name="solver_lhs5" localSheetId="1" hidden="1">'Blending Problem'!$G$22</definedName>
+    <definedName name="solver_lhs5" localSheetId="2" hidden="1">'Marketing Research'!$H$18</definedName>
+    <definedName name="solver_lhs5" localSheetId="3" hidden="1">'Media Selection'!$G$18</definedName>
     <definedName name="solver_lhs5" localSheetId="0" hidden="1">'Portfolio Selection'!$E$32</definedName>
-    <definedName name="solver_lhs6" localSheetId="1" hidden="1">'Blending Problem'!$G$26:$G$27</definedName>
-    <definedName name="solver_lhs6" localSheetId="3" hidden="1">'Media Selection'!$G$27:$G$29</definedName>
-    <definedName name="solver_lhs7" localSheetId="1" hidden="1">'Blending Problem'!$G$27</definedName>
-    <definedName name="solver_lhs8" localSheetId="1" hidden="1">'Blending Problem'!$G$27</definedName>
+    <definedName name="solver_lhs6" localSheetId="1" hidden="1">'Blending Problem'!$G$23</definedName>
+    <definedName name="solver_lhs6" localSheetId="2" hidden="1">'Marketing Research'!$H$19</definedName>
+    <definedName name="solver_lhs6" localSheetId="3" hidden="1">'Media Selection'!$G$19</definedName>
+    <definedName name="solver_lhs7" localSheetId="1" hidden="1">'Blending Problem'!$G$24</definedName>
+    <definedName name="solver_lhs7" localSheetId="3" hidden="1">'Media Selection'!$G$20</definedName>
+    <definedName name="solver_lhs8" localSheetId="1" hidden="1">'Blending Problem'!$G$25</definedName>
+    <definedName name="solver_lhs8" localSheetId="3" hidden="1">'Media Selection'!$G$21</definedName>
+    <definedName name="solver_lhs9" localSheetId="1" hidden="1">'Blending Problem'!$G$26</definedName>
+    <definedName name="solver_lhs9" localSheetId="3" hidden="1">'Media Selection'!$G$22</definedName>
     <definedName name="solver_lin" localSheetId="1" hidden="1">2</definedName>
     <definedName name="solver_lin" localSheetId="2" hidden="1">2</definedName>
     <definedName name="solver_lin" localSheetId="3" hidden="1">2</definedName>
@@ -165,10 +184,10 @@
     <definedName name="solver_nod" localSheetId="2" hidden="1">2147483647</definedName>
     <definedName name="solver_nod" localSheetId="3" hidden="1">2147483647</definedName>
     <definedName name="solver_nod" localSheetId="0" hidden="1">2147483647</definedName>
-    <definedName name="solver_num" localSheetId="1" hidden="1">0</definedName>
-    <definedName name="solver_num" localSheetId="2" hidden="1">0</definedName>
-    <definedName name="solver_num" localSheetId="3" hidden="1">0</definedName>
-    <definedName name="solver_num" localSheetId="0" hidden="1">0</definedName>
+    <definedName name="solver_num" localSheetId="1" hidden="1">10</definedName>
+    <definedName name="solver_num" localSheetId="2" hidden="1">6</definedName>
+    <definedName name="solver_num" localSheetId="3" hidden="1">16</definedName>
+    <definedName name="solver_num" localSheetId="0" hidden="1">5</definedName>
     <definedName name="solver_nwt" localSheetId="1" hidden="1">1</definedName>
     <definedName name="solver_nwt" localSheetId="2" hidden="1">1</definedName>
     <definedName name="solver_nwt" localSheetId="3" hidden="1">1</definedName>
@@ -176,10 +195,10 @@
     <definedName name="solver_ofx" localSheetId="1" hidden="1">2</definedName>
     <definedName name="solver_ofx" localSheetId="2" hidden="1">2</definedName>
     <definedName name="solver_ofx" localSheetId="0" hidden="1">2</definedName>
-    <definedName name="solver_opt" localSheetId="1" hidden="1">'Blending Problem'!$H$32</definedName>
-    <definedName name="solver_opt" localSheetId="2" hidden="1">'Marketing Research'!$H$27</definedName>
-    <definedName name="solver_opt" localSheetId="3" hidden="1">'Media Selection'!$H$34</definedName>
-    <definedName name="solver_opt" localSheetId="0" hidden="1">'Portfolio Selection'!$G$40</definedName>
+    <definedName name="solver_opt" localSheetId="1" hidden="1">'Blending Problem'!$G$15</definedName>
+    <definedName name="solver_opt" localSheetId="2" hidden="1">'Marketing Research'!$H$11</definedName>
+    <definedName name="solver_opt" localSheetId="3" hidden="1">'Media Selection'!$G$9</definedName>
+    <definedName name="solver_opt" localSheetId="0" hidden="1">'Portfolio Selection'!$E$25</definedName>
     <definedName name="solver_piv" localSheetId="1" hidden="1">0.000001</definedName>
     <definedName name="solver_piv" localSheetId="2" hidden="1">0.000001</definedName>
     <definedName name="solver_piv" localSheetId="0" hidden="1">0.000001</definedName>
@@ -198,55 +217,85 @@
     <definedName name="solver_red" localSheetId="2" hidden="1">0.000001</definedName>
     <definedName name="solver_red" localSheetId="0" hidden="1">0.000001</definedName>
     <definedName name="solver_rel1" localSheetId="1" hidden="1">1</definedName>
-    <definedName name="solver_rel1" localSheetId="2" hidden="1">4</definedName>
+    <definedName name="solver_rel1" localSheetId="2" hidden="1">2</definedName>
     <definedName name="solver_rel1" localSheetId="3" hidden="1">3</definedName>
     <definedName name="solver_rel1" localSheetId="0" hidden="1">1</definedName>
-    <definedName name="solver_rel2" localSheetId="1" hidden="1">3</definedName>
-    <definedName name="solver_rel2" localSheetId="2" hidden="1">2</definedName>
-    <definedName name="solver_rel2" localSheetId="3" hidden="1">1</definedName>
-    <definedName name="solver_rel2" localSheetId="0" hidden="1">3</definedName>
+    <definedName name="solver_rel10" localSheetId="1" hidden="1">3</definedName>
+    <definedName name="solver_rel10" localSheetId="3" hidden="1">1</definedName>
+    <definedName name="solver_rel11" localSheetId="3" hidden="1">3</definedName>
+    <definedName name="solver_rel12" localSheetId="3" hidden="1">3</definedName>
+    <definedName name="solver_rel13" localSheetId="3" hidden="1">3</definedName>
+    <definedName name="solver_rel14" localSheetId="3" hidden="1">1</definedName>
+    <definedName name="solver_rel15" localSheetId="3" hidden="1">1</definedName>
+    <definedName name="solver_rel16" localSheetId="3" hidden="1">1</definedName>
+    <definedName name="solver_rel2" localSheetId="1" hidden="1">1</definedName>
+    <definedName name="solver_rel2" localSheetId="2" hidden="1">3</definedName>
+    <definedName name="solver_rel2" localSheetId="3" hidden="1">3</definedName>
+    <definedName name="solver_rel2" localSheetId="0" hidden="1">1</definedName>
     <definedName name="solver_rel3" localSheetId="1" hidden="1">1</definedName>
     <definedName name="solver_rel3" localSheetId="2" hidden="1">3</definedName>
     <definedName name="solver_rel3" localSheetId="3" hidden="1">3</definedName>
     <definedName name="solver_rel3" localSheetId="0" hidden="1">1</definedName>
-    <definedName name="solver_rel4" localSheetId="1" hidden="1">3</definedName>
+    <definedName name="solver_rel4" localSheetId="1" hidden="1">1</definedName>
+    <definedName name="solver_rel4" localSheetId="2" hidden="1">3</definedName>
     <definedName name="solver_rel4" localSheetId="3" hidden="1">1</definedName>
     <definedName name="solver_rel4" localSheetId="0" hidden="1">3</definedName>
-    <definedName name="solver_rel5" localSheetId="1" hidden="1">1</definedName>
-    <definedName name="solver_rel5" localSheetId="3" hidden="1">3</definedName>
+    <definedName name="solver_rel5" localSheetId="1" hidden="1">3</definedName>
+    <definedName name="solver_rel5" localSheetId="2" hidden="1">3</definedName>
+    <definedName name="solver_rel5" localSheetId="3" hidden="1">1</definedName>
     <definedName name="solver_rel5" localSheetId="0" hidden="1">1</definedName>
-    <definedName name="solver_rel6" localSheetId="1" hidden="1">3</definedName>
+    <definedName name="solver_rel6" localSheetId="1" hidden="1">1</definedName>
+    <definedName name="solver_rel6" localSheetId="2" hidden="1">3</definedName>
     <definedName name="solver_rel6" localSheetId="3" hidden="1">1</definedName>
     <definedName name="solver_rel7" localSheetId="1" hidden="1">3</definedName>
-    <definedName name="solver_rel8" localSheetId="1" hidden="1">3</definedName>
+    <definedName name="solver_rel7" localSheetId="3" hidden="1">1</definedName>
+    <definedName name="solver_rel8" localSheetId="1" hidden="1">1</definedName>
+    <definedName name="solver_rel8" localSheetId="3" hidden="1">1</definedName>
+    <definedName name="solver_rel9" localSheetId="1" hidden="1">3</definedName>
+    <definedName name="solver_rel9" localSheetId="3" hidden="1">1</definedName>
     <definedName name="solver_reo" localSheetId="1" hidden="1">2</definedName>
     <definedName name="solver_reo" localSheetId="2" hidden="1">2</definedName>
     <definedName name="solver_reo" localSheetId="0" hidden="1">2</definedName>
     <definedName name="solver_rep" localSheetId="1" hidden="1">2</definedName>
     <definedName name="solver_rep" localSheetId="2" hidden="1">2</definedName>
     <definedName name="solver_rep" localSheetId="0" hidden="1">2</definedName>
-    <definedName name="solver_rhs1" localSheetId="1" hidden="1">'Blending Problem'!$I$18:$I$21</definedName>
-    <definedName name="solver_rhs1" localSheetId="2" hidden="1">"integer"</definedName>
-    <definedName name="solver_rhs1" localSheetId="3" hidden="1">'Media Selection'!$I$14:$I$16</definedName>
-    <definedName name="solver_rhs1" localSheetId="0" hidden="1">'Portfolio Selection'!$G$28:$G$30</definedName>
-    <definedName name="solver_rhs2" localSheetId="1" hidden="1">'Blending Problem'!$I$22</definedName>
-    <definedName name="solver_rhs2" localSheetId="2" hidden="1">'Marketing Research'!$J$14</definedName>
-    <definedName name="solver_rhs2" localSheetId="3" hidden="1">'Media Selection'!$I$17:$I$23</definedName>
-    <definedName name="solver_rhs2" localSheetId="0" hidden="1">'Portfolio Selection'!$G$31</definedName>
-    <definedName name="solver_rhs3" localSheetId="1" hidden="1">'Blending Problem'!$I$23</definedName>
-    <definedName name="solver_rhs3" localSheetId="2" hidden="1">'Marketing Research'!$J$15:$J$19</definedName>
-    <definedName name="solver_rhs3" localSheetId="3" hidden="1">'Media Selection'!$I$24:$I$26</definedName>
-    <definedName name="solver_rhs3" localSheetId="0" hidden="1">'Portfolio Selection'!$G$32</definedName>
-    <definedName name="solver_rhs4" localSheetId="1" hidden="1">'Blending Problem'!$I$24</definedName>
-    <definedName name="solver_rhs4" localSheetId="3" hidden="1">'Media Selection'!$I$27:$I$29</definedName>
+    <definedName name="solver_rhs1" localSheetId="1" hidden="1">'Blending Problem'!$I$18</definedName>
+    <definedName name="solver_rhs1" localSheetId="2" hidden="1">'Marketing Research'!$J$14</definedName>
+    <definedName name="solver_rhs1" localSheetId="3" hidden="1">'Media Selection'!$I$14</definedName>
+    <definedName name="solver_rhs1" localSheetId="0" hidden="1">'Portfolio Selection'!$G$28</definedName>
+    <definedName name="solver_rhs10" localSheetId="1" hidden="1">'Blending Problem'!$I$27</definedName>
+    <definedName name="solver_rhs10" localSheetId="3" hidden="1">'Media Selection'!$I$23</definedName>
+    <definedName name="solver_rhs11" localSheetId="3" hidden="1">'Media Selection'!$I$24</definedName>
+    <definedName name="solver_rhs12" localSheetId="3" hidden="1">'Media Selection'!$I$25</definedName>
+    <definedName name="solver_rhs13" localSheetId="3" hidden="1">'Media Selection'!$I$26</definedName>
+    <definedName name="solver_rhs14" localSheetId="3" hidden="1">'Media Selection'!$I$27</definedName>
+    <definedName name="solver_rhs15" localSheetId="3" hidden="1">'Media Selection'!$I$28</definedName>
+    <definedName name="solver_rhs16" localSheetId="3" hidden="1">'Media Selection'!$I$29</definedName>
+    <definedName name="solver_rhs2" localSheetId="1" hidden="1">'Blending Problem'!$I$19</definedName>
+    <definedName name="solver_rhs2" localSheetId="2" hidden="1">'Marketing Research'!$J$15</definedName>
+    <definedName name="solver_rhs2" localSheetId="3" hidden="1">'Media Selection'!$I$15</definedName>
+    <definedName name="solver_rhs2" localSheetId="0" hidden="1">'Portfolio Selection'!$G$29</definedName>
+    <definedName name="solver_rhs3" localSheetId="1" hidden="1">'Blending Problem'!$I$20</definedName>
+    <definedName name="solver_rhs3" localSheetId="2" hidden="1">'Marketing Research'!$J$16</definedName>
+    <definedName name="solver_rhs3" localSheetId="3" hidden="1">'Media Selection'!$I$16</definedName>
+    <definedName name="solver_rhs3" localSheetId="0" hidden="1">'Portfolio Selection'!$G$30</definedName>
+    <definedName name="solver_rhs4" localSheetId="1" hidden="1">'Blending Problem'!$I$21</definedName>
+    <definedName name="solver_rhs4" localSheetId="2" hidden="1">'Marketing Research'!$J$17</definedName>
+    <definedName name="solver_rhs4" localSheetId="3" hidden="1">'Media Selection'!$I$17</definedName>
     <definedName name="solver_rhs4" localSheetId="0" hidden="1">'Portfolio Selection'!$G$31</definedName>
-    <definedName name="solver_rhs5" localSheetId="1" hidden="1">'Blending Problem'!$I$25</definedName>
-    <definedName name="solver_rhs5" localSheetId="3" hidden="1">'Media Selection'!$I$24:$I$26</definedName>
+    <definedName name="solver_rhs5" localSheetId="1" hidden="1">'Blending Problem'!$I$22</definedName>
+    <definedName name="solver_rhs5" localSheetId="2" hidden="1">'Marketing Research'!$J$18</definedName>
+    <definedName name="solver_rhs5" localSheetId="3" hidden="1">'Media Selection'!$I$18</definedName>
     <definedName name="solver_rhs5" localSheetId="0" hidden="1">'Portfolio Selection'!$G$32</definedName>
-    <definedName name="solver_rhs6" localSheetId="1" hidden="1">'Blending Problem'!$I$26:$I$27</definedName>
-    <definedName name="solver_rhs6" localSheetId="3" hidden="1">'Media Selection'!$I$27:$I$29</definedName>
-    <definedName name="solver_rhs7" localSheetId="1" hidden="1">'Blending Problem'!$I$27</definedName>
-    <definedName name="solver_rhs8" localSheetId="1" hidden="1">'Blending Problem'!$I$27</definedName>
+    <definedName name="solver_rhs6" localSheetId="1" hidden="1">'Blending Problem'!$I$23</definedName>
+    <definedName name="solver_rhs6" localSheetId="2" hidden="1">'Marketing Research'!$J$19</definedName>
+    <definedName name="solver_rhs6" localSheetId="3" hidden="1">'Media Selection'!$I$19</definedName>
+    <definedName name="solver_rhs7" localSheetId="1" hidden="1">'Blending Problem'!$I$24</definedName>
+    <definedName name="solver_rhs7" localSheetId="3" hidden="1">'Media Selection'!$I$20</definedName>
+    <definedName name="solver_rhs8" localSheetId="1" hidden="1">'Blending Problem'!$I$25</definedName>
+    <definedName name="solver_rhs8" localSheetId="3" hidden="1">'Media Selection'!$I$21</definedName>
+    <definedName name="solver_rhs9" localSheetId="1" hidden="1">'Blending Problem'!$I$26</definedName>
+    <definedName name="solver_rhs9" localSheetId="3" hidden="1">'Media Selection'!$I$22</definedName>
     <definedName name="solver_rlx" localSheetId="1" hidden="1">2</definedName>
     <definedName name="solver_rlx" localSheetId="2" hidden="1">2</definedName>
     <definedName name="solver_rlx" localSheetId="3" hidden="1">2</definedName>
@@ -279,17 +328,17 @@
     <definedName name="solver_tol" localSheetId="3" hidden="1">0.01</definedName>
     <definedName name="solver_tol" localSheetId="0" hidden="1">0.01</definedName>
     <definedName name="solver_typ" localSheetId="1" hidden="1">1</definedName>
-    <definedName name="solver_typ" localSheetId="2" hidden="1">1</definedName>
+    <definedName name="solver_typ" localSheetId="2" hidden="1">2</definedName>
     <definedName name="solver_typ" localSheetId="3" hidden="1">1</definedName>
     <definedName name="solver_typ" localSheetId="0" hidden="1">1</definedName>
     <definedName name="solver_val" localSheetId="1" hidden="1">0</definedName>
     <definedName name="solver_val" localSheetId="2" hidden="1">0</definedName>
     <definedName name="solver_val" localSheetId="3" hidden="1">0</definedName>
     <definedName name="solver_val" localSheetId="0" hidden="1">0</definedName>
-    <definedName name="solver_ver" localSheetId="1" hidden="1">2</definedName>
-    <definedName name="solver_ver" localSheetId="2" hidden="1">2</definedName>
-    <definedName name="solver_ver" localSheetId="3" hidden="1">2</definedName>
-    <definedName name="solver_ver" localSheetId="0" hidden="1">2</definedName>
+    <definedName name="solver_ver" localSheetId="1" hidden="1">3</definedName>
+    <definedName name="solver_ver" localSheetId="2" hidden="1">3</definedName>
+    <definedName name="solver_ver" localSheetId="3" hidden="1">3</definedName>
+    <definedName name="solver_ver" localSheetId="0" hidden="1">3</definedName>
     <definedName name="sssolver_cvg" localSheetId="2" hidden="1">0.0001</definedName>
     <definedName name="sssolver_drv" localSheetId="1" hidden="1">1</definedName>
     <definedName name="sssolver_drv" localSheetId="2" hidden="1">1</definedName>
@@ -975,7 +1024,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="119">
   <si>
     <t>Interview Cost ($)</t>
   </si>
@@ -1326,6 +1375,21 @@
   <si>
     <t>Min amount
 (in gallons)</t>
+  </si>
+  <si>
+    <t>&lt;=</t>
+  </si>
+  <si>
+    <t>&gt;=</t>
+  </si>
+  <si>
+    <t>&gt;</t>
+  </si>
+  <si>
+    <t>&lt;</t>
+  </si>
+  <si>
+    <t>=</t>
   </si>
 </sst>
 </file>
@@ -1678,7 +1742,7 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="3" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
     <cellStyle name="Normal 3" xfId="4" xr:uid="{00000000-0005-0000-0000-000004000000}"/>
-    <cellStyle name="Per cent" xfId="5" builtinId="5"/>
+    <cellStyle name="Percent" xfId="5" builtinId="5"/>
   </cellStyles>
   <dxfs count="2">
     <dxf>
@@ -16258,10 +16322,6 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -16527,23 +16587,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A16:G32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="G51" sqref="G51"/>
+    <sheetView topLeftCell="A18" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G26" sqref="G26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.83203125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="17.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.1640625" style="1"/>
-    <col min="4" max="4" width="43.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.83203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="16384" width="9.1640625" style="1"/>
+    <col min="1" max="1" width="18.85546875" style="1" customWidth="1"/>
+    <col min="2" max="2" width="17.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.140625" style="1"/>
+    <col min="4" max="4" width="43.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="51" t="s">
         <v>102</v>
       </c>
@@ -16553,7 +16613,7 @@
       <c r="E16" s="51"/>
       <c r="F16" s="4"/>
     </row>
-    <row r="17" spans="1:7" s="18" customFormat="1" ht="34" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:7" s="18" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A17" s="17" t="s">
         <v>52</v>
       </c>
@@ -16561,7 +16621,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="9" t="s">
         <v>53</v>
       </c>
@@ -16576,7 +16636,7 @@
         <v>100000</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="9" t="s">
         <v>55</v>
       </c>
@@ -16590,7 +16650,7 @@
         <v>50000</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="9" t="s">
         <v>56</v>
       </c>
@@ -16604,7 +16664,7 @@
         <v>50000</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="9" t="s">
         <v>57</v>
       </c>
@@ -16619,7 +16679,7 @@
       </c>
       <c r="F21"/>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="9" t="s">
         <v>58</v>
       </c>
@@ -16634,13 +16694,13 @@
       </c>
       <c r="F22"/>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23"/>
       <c r="B23"/>
       <c r="E23"/>
       <c r="F23"/>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="51" t="s">
         <v>105</v>
       </c>
@@ -16650,7 +16710,7 @@
       </c>
       <c r="E24" s="51"/>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="17"/>
       <c r="B25" s="4" t="s">
         <v>59</v>
@@ -16658,21 +16718,28 @@
       <c r="D25" s="8" t="s">
         <v>60</v>
       </c>
-      <c r="E25" s="30"/>
+      <c r="E25" s="30">
+        <f>SUM(0.073*B26+0.103*B27+0.064*B28+0.075*B29+0.045*B30)</f>
+        <v>8000</v>
+      </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" s="8" t="s">
         <v>62</v>
       </c>
-      <c r="B26" s="29"/>
+      <c r="B26" s="29">
+        <v>20000</v>
+      </c>
       <c r="D26" s="4"/>
       <c r="E26"/>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" s="8" t="s">
         <v>63</v>
       </c>
-      <c r="B27" s="29"/>
+      <c r="B27" s="29">
+        <v>30000</v>
+      </c>
       <c r="D27" s="51" t="s">
         <v>108</v>
       </c>
@@ -16680,59 +16747,105 @@
       <c r="F27" s="51"/>
       <c r="G27" s="51"/>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" s="8" t="s">
         <v>64</v>
       </c>
-      <c r="B28" s="29"/>
+      <c r="B28" s="29">
+        <v>0</v>
+      </c>
       <c r="D28" s="21" t="s">
         <v>78</v>
       </c>
-      <c r="E28" s="29"/>
-      <c r="F28" s="16"/>
-      <c r="G28" s="29"/>
+      <c r="E28" s="29">
+        <f>SUM(B26:B30)</f>
+        <v>100000</v>
+      </c>
+      <c r="F28" s="16" t="s">
+        <v>114</v>
+      </c>
+      <c r="G28" s="29">
+        <f>E18</f>
+        <v>100000</v>
+      </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" s="8" t="s">
         <v>65</v>
       </c>
-      <c r="B29" s="29"/>
+      <c r="B29" s="29">
+        <v>40000</v>
+      </c>
       <c r="D29" s="21" t="s">
         <v>79</v>
       </c>
-      <c r="E29" s="29"/>
-      <c r="F29" s="16"/>
-      <c r="G29" s="29"/>
+      <c r="E29" s="29">
+        <f>SUM(B26:B27)</f>
+        <v>50000</v>
+      </c>
+      <c r="F29" s="16" t="s">
+        <v>114</v>
+      </c>
+      <c r="G29" s="29">
+        <f>E19</f>
+        <v>50000</v>
+      </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" s="8" t="s">
         <v>66</v>
       </c>
-      <c r="B30" s="29"/>
+      <c r="B30" s="29">
+        <v>10000</v>
+      </c>
       <c r="D30" s="21" t="s">
         <v>80</v>
       </c>
-      <c r="E30" s="29"/>
-      <c r="F30" s="16"/>
-      <c r="G30" s="29"/>
+      <c r="E30" s="29">
+        <f>SUM(B28:B29)</f>
+        <v>40000</v>
+      </c>
+      <c r="F30" s="16" t="s">
+        <v>114</v>
+      </c>
+      <c r="G30" s="29">
+        <f>E20</f>
+        <v>50000</v>
+      </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="D31" s="21" t="s">
         <v>81</v>
       </c>
-      <c r="E31" s="29"/>
-      <c r="F31" s="16"/>
-      <c r="G31" s="29"/>
+      <c r="E31" s="29">
+        <f>B30</f>
+        <v>10000</v>
+      </c>
+      <c r="F31" s="16" t="s">
+        <v>115</v>
+      </c>
+      <c r="G31" s="29">
+        <f>0.25*E30</f>
+        <v>10000</v>
+      </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32"/>
       <c r="B32"/>
       <c r="D32" s="21" t="s">
         <v>82</v>
       </c>
-      <c r="E32" s="29"/>
-      <c r="F32" s="16"/>
-      <c r="G32" s="29"/>
+      <c r="E32" s="29">
+        <f>B27</f>
+        <v>30000</v>
+      </c>
+      <c r="F32" s="16" t="s">
+        <v>114</v>
+      </c>
+      <c r="G32" s="29">
+        <f>0.6*(B26+B27)</f>
+        <v>30000</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -16757,25 +16870,25 @@
   </sheetPr>
   <dimension ref="A1:J28"/>
   <sheetViews>
-    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="H32" sqref="H32"/>
+    <sheetView topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.7109375" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="18" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="20.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.6640625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="13.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.7109375" style="1" customWidth="1"/>
+    <col min="5" max="5" width="13.42578125" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="20" style="1" customWidth="1"/>
-    <col min="7" max="7" width="10.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.83203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.1640625" style="1" customWidth="1"/>
-    <col min="10" max="16384" width="9.1640625" style="1"/>
+    <col min="7" max="7" width="10.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.140625" style="1" customWidth="1"/>
+    <col min="10" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="51" t="s">
         <v>109</v>
       </c>
@@ -16785,7 +16898,7 @@
       <c r="E1" s="51"/>
       <c r="F1" s="51"/>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="57" t="s">
         <v>67</v>
       </c>
@@ -16795,7 +16908,7 @@
       </c>
       <c r="F2" s="57"/>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>68</v>
       </c>
@@ -16809,7 +16922,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>70</v>
       </c>
@@ -16824,7 +16937,7 @@
       </c>
       <c r="J4" s="6"/>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="E5" s="8" t="s">
         <v>71</v>
       </c>
@@ -16832,7 +16945,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="6" spans="1:10" ht="34" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:10" ht="31.5" x14ac:dyDescent="0.25">
       <c r="B6" s="2"/>
       <c r="C6" s="2"/>
       <c r="D6" s="2"/>
@@ -16843,13 +16956,13 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B7" s="2"/>
       <c r="C7" s="2"/>
       <c r="D7" s="2"/>
       <c r="E7" s="8"/>
     </row>
-    <row r="8" spans="1:10" ht="34" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:10" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
         <v>77</v>
       </c>
@@ -16865,7 +16978,7 @@
       </c>
       <c r="F8" s="57"/>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="6">
         <v>1</v>
       </c>
@@ -16883,7 +16996,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="6">
         <v>2</v>
       </c>
@@ -16901,7 +17014,7 @@
         <v>0.45</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="4">
         <v>3</v>
       </c>
@@ -16919,14 +17032,14 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="12" spans="1:10" ht="18" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A12" s="23"/>
       <c r="E12"/>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="E13"/>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="58" t="s">
         <v>21</v>
       </c>
@@ -16938,7 +17051,7 @@
       </c>
       <c r="G14" s="58"/>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="16"/>
       <c r="B15" s="16" t="s">
         <v>83</v>
@@ -16950,26 +17063,37 @@
       <c r="F15" s="8" t="s">
         <v>76</v>
       </c>
-      <c r="G15" s="35"/>
+      <c r="G15" s="35">
+        <f>SUM(0.4*B16+0.3*B17+0.06*B18+0.5*C16+0.4*C17+0.16*C18)</f>
+        <v>7099.9999999999991</v>
+      </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" s="32" t="s">
         <v>99</v>
       </c>
-      <c r="B16" s="39"/>
-      <c r="C16" s="41"/>
+      <c r="B16" s="39">
+        <v>1250.0000000000005</v>
+      </c>
+      <c r="C16" s="41">
+        <v>3749.9999999999986</v>
+      </c>
       <c r="D16"/>
       <c r="E16"/>
       <c r="F16" s="8"/>
       <c r="G16" s="31"/>
       <c r="H16" s="31"/>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" s="32" t="s">
         <v>100</v>
       </c>
-      <c r="B17" s="39"/>
-      <c r="C17" s="41"/>
+      <c r="B17" s="39">
+        <v>6750.0000000000027</v>
+      </c>
+      <c r="C17" s="41">
+        <v>3249.9999999999973</v>
+      </c>
       <c r="D17"/>
       <c r="E17" s="55" t="s">
         <v>110</v>
@@ -16979,22 +17103,34 @@
       <c r="H17" s="55"/>
       <c r="I17" s="55"/>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" s="32" t="s">
         <v>101</v>
       </c>
-      <c r="B18" s="39"/>
-      <c r="C18" s="41"/>
+      <c r="B18" s="39">
+        <v>2000.0000000000009</v>
+      </c>
+      <c r="C18" s="41">
+        <v>7999.9999999999982</v>
+      </c>
       <c r="D18"/>
       <c r="E18" s="56" t="s">
         <v>89</v>
       </c>
       <c r="F18" s="56"/>
-      <c r="G18" s="36"/>
-      <c r="H18" s="10"/>
-      <c r="I18" s="36"/>
+      <c r="G18" s="36">
+        <f>SUM(B16:C16)</f>
+        <v>4999.9999999999991</v>
+      </c>
+      <c r="H18" s="10" t="s">
+        <v>114</v>
+      </c>
+      <c r="I18" s="36">
+        <f>C9</f>
+        <v>5000</v>
+      </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" s="10"/>
       <c r="B19" s="8"/>
       <c r="C19" s="13"/>
@@ -17003,11 +17139,19 @@
         <v>90</v>
       </c>
       <c r="F19" s="52"/>
-      <c r="G19" s="36"/>
-      <c r="H19" s="10"/>
-      <c r="I19" s="36"/>
+      <c r="G19" s="36">
+        <f>SUM(B17:C17)</f>
+        <v>10000</v>
+      </c>
+      <c r="H19" s="10" t="s">
+        <v>114</v>
+      </c>
+      <c r="I19" s="36">
+        <f>C10</f>
+        <v>10000</v>
+      </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" s="42"/>
       <c r="B20" s="32"/>
       <c r="C20"/>
@@ -17016,11 +17160,19 @@
         <v>91</v>
       </c>
       <c r="F20" s="52"/>
-      <c r="G20" s="36"/>
-      <c r="H20" s="10"/>
-      <c r="I20" s="36"/>
+      <c r="G20" s="36">
+        <f>SUM(B18:C18)</f>
+        <v>10000</v>
+      </c>
+      <c r="H20" s="10" t="s">
+        <v>114</v>
+      </c>
+      <c r="I20" s="36">
+        <f>C11</f>
+        <v>10000</v>
+      </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" s="43"/>
       <c r="B21" s="32"/>
       <c r="C21"/>
@@ -17031,11 +17183,19 @@
       <c r="F21" s="8" t="s">
         <v>92</v>
       </c>
-      <c r="G21" s="37"/>
-      <c r="H21" s="8"/>
-      <c r="I21" s="37"/>
+      <c r="G21" s="37">
+        <f>B16</f>
+        <v>1250.0000000000005</v>
+      </c>
+      <c r="H21" s="8" t="s">
+        <v>114</v>
+      </c>
+      <c r="I21" s="37">
+        <f>0.3*SUM(B16:B18)</f>
+        <v>3000.0000000000009</v>
+      </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" s="43"/>
       <c r="B22" s="32"/>
       <c r="C22"/>
@@ -17044,11 +17204,19 @@
       <c r="F22" s="8" t="s">
         <v>93</v>
       </c>
-      <c r="G22" s="37"/>
-      <c r="H22" s="8"/>
-      <c r="I22" s="37"/>
+      <c r="G22" s="37">
+        <f t="shared" ref="G22:G23" si="0">B17</f>
+        <v>6750.0000000000027</v>
+      </c>
+      <c r="H22" s="8" t="s">
+        <v>116</v>
+      </c>
+      <c r="I22" s="37">
+        <f>0.4*SUM(B16:B18)</f>
+        <v>4000.0000000000018</v>
+      </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23"/>
       <c r="B23"/>
       <c r="C23"/>
@@ -17057,49 +17225,89 @@
       <c r="F23" s="8" t="s">
         <v>94</v>
       </c>
-      <c r="G23" s="37"/>
-      <c r="H23" s="8"/>
-      <c r="I23" s="37"/>
+      <c r="G23" s="37">
+        <f t="shared" si="0"/>
+        <v>2000.0000000000009</v>
+      </c>
+      <c r="H23" s="8" t="s">
+        <v>117</v>
+      </c>
+      <c r="I23" s="37">
+        <f>0.2*SUM(B16:B18)</f>
+        <v>2000.0000000000009</v>
+      </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="E24" s="54" t="s">
         <v>88</v>
       </c>
       <c r="F24" s="8" t="s">
         <v>95</v>
       </c>
-      <c r="G24" s="37"/>
-      <c r="H24" s="8"/>
-      <c r="I24" s="37"/>
+      <c r="G24" s="37">
+        <f>C16</f>
+        <v>3749.9999999999986</v>
+      </c>
+      <c r="H24" s="8" t="s">
+        <v>116</v>
+      </c>
+      <c r="I24" s="37">
+        <f>0.25*SUM(C16:C18)</f>
+        <v>3749.9999999999986</v>
+      </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="E25" s="52"/>
       <c r="F25" s="8" t="s">
         <v>96</v>
       </c>
-      <c r="G25" s="37"/>
-      <c r="H25" s="8"/>
-      <c r="I25" s="37"/>
+      <c r="G25" s="37">
+        <f t="shared" ref="G25:G26" si="1">C17</f>
+        <v>3249.9999999999973</v>
+      </c>
+      <c r="H25" s="8" t="s">
+        <v>117</v>
+      </c>
+      <c r="I25" s="37">
+        <f>0.45*SUM(C16:C18)</f>
+        <v>6749.9999999999973</v>
+      </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="E26" s="52"/>
       <c r="F26" s="8" t="s">
         <v>97</v>
       </c>
-      <c r="G26" s="37"/>
-      <c r="H26" s="8"/>
-      <c r="I26" s="37"/>
+      <c r="G26" s="37">
+        <f t="shared" si="1"/>
+        <v>7999.9999999999982</v>
+      </c>
+      <c r="H26" s="8" t="s">
+        <v>116</v>
+      </c>
+      <c r="I26" s="37">
+        <f>0.3*SUM(C16:C18)</f>
+        <v>4499.9999999999982</v>
+      </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="E27" s="53" t="s">
         <v>98</v>
       </c>
       <c r="F27" s="53"/>
-      <c r="G27" s="38"/>
-      <c r="H27" s="9"/>
-      <c r="I27" s="38"/>
+      <c r="G27" s="38">
+        <f>SUM(B16:B18)</f>
+        <v>10000.000000000004</v>
+      </c>
+      <c r="H27" s="9" t="s">
+        <v>116</v>
+      </c>
+      <c r="I27" s="38">
+        <f>F6</f>
+        <v>10000</v>
+      </c>
     </row>
-    <row r="28" spans="1:9" ht="33" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="28" spans="1:9" ht="33" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="13">
     <mergeCell ref="A1:F1"/>
@@ -17132,24 +17340,24 @@
   </sheetPr>
   <dimension ref="A1:J19"/>
   <sheetViews>
-    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="H27" sqref="H27"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H14" sqref="H14:J19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.5" style="1" customWidth="1"/>
-    <col min="2" max="2" width="10.83203125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="13.1640625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="10.33203125" style="1" customWidth="1"/>
-    <col min="5" max="5" width="10.1640625" style="1" customWidth="1"/>
-    <col min="6" max="6" width="16.33203125" style="1" customWidth="1"/>
-    <col min="7" max="7" width="18.5" style="1" customWidth="1"/>
-    <col min="8" max="8" width="29.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="16384" width="8.83203125" style="1"/>
+    <col min="1" max="1" width="15.42578125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="10.85546875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="13.140625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="10.28515625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="10.140625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="16.28515625" style="1" customWidth="1"/>
+    <col min="7" max="7" width="18.42578125" style="1" customWidth="1"/>
+    <col min="8" max="8" width="29.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="16384" width="8.85546875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="51" t="s">
         <v>109</v>
       </c>
@@ -17162,13 +17370,13 @@
       <c r="H1" s="51"/>
       <c r="I1" s="51"/>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B2" s="2" t="s">
         <v>0</v>
       </c>
       <c r="C2" s="3"/>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>1</v>
       </c>
@@ -17185,7 +17393,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>5</v>
       </c>
@@ -17202,7 +17410,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>7</v>
       </c>
@@ -17219,7 +17427,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="H6" s="6" t="s">
         <v>9</v>
       </c>
@@ -17227,7 +17435,7 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="H7" s="6" t="s">
         <v>10</v>
       </c>
@@ -17235,10 +17443,10 @@
         <v>0.6</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="4"/>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="51" t="s">
         <v>19</v>
       </c>
@@ -17250,7 +17458,7 @@
       </c>
       <c r="H10" s="51"/>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="20"/>
       <c r="B11" s="60" t="s">
         <v>20</v>
@@ -17260,9 +17468,12 @@
       <c r="G11" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="H11" s="29"/>
+      <c r="H11" s="29">
+        <f>SUM(B4*B13+C4*C13+B5*B14+C5*C14)</f>
+        <v>20320</v>
+      </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
         <v>1</v>
       </c>
@@ -17276,12 +17487,16 @@
       <c r="F12" s="4"/>
       <c r="G12" s="13"/>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B13" s="7"/>
-      <c r="C13" s="7"/>
+      <c r="B13" s="7">
+        <v>240</v>
+      </c>
+      <c r="C13" s="7">
+        <v>160</v>
+      </c>
       <c r="F13" s="58" t="s">
         <v>110</v>
       </c>
@@ -17290,65 +17505,117 @@
       <c r="I13" s="58"/>
       <c r="J13" s="58"/>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B14" s="7"/>
-      <c r="C14" s="7"/>
+      <c r="B14" s="7">
+        <v>240</v>
+      </c>
+      <c r="C14" s="7">
+        <v>360</v>
+      </c>
       <c r="F14" s="61" t="s">
         <v>13</v>
       </c>
       <c r="G14" s="61"/>
-      <c r="H14" s="7"/>
-      <c r="I14" s="50"/>
-      <c r="J14" s="7"/>
+      <c r="H14" s="7">
+        <f>SUM(B13:C14)</f>
+        <v>1000</v>
+      </c>
+      <c r="I14" s="50" t="s">
+        <v>118</v>
+      </c>
+      <c r="J14" s="7">
+        <f>I3</f>
+        <v>1000</v>
+      </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="4"/>
       <c r="F15" s="59" t="s">
         <v>14</v>
       </c>
       <c r="G15" s="59"/>
-      <c r="H15" s="7"/>
-      <c r="I15" s="16"/>
-      <c r="J15" s="7"/>
+      <c r="H15" s="7">
+        <f>SUM(B13:C13)</f>
+        <v>400</v>
+      </c>
+      <c r="I15" s="16" t="s">
+        <v>115</v>
+      </c>
+      <c r="J15" s="7">
+        <f>I4</f>
+        <v>400</v>
+      </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="F16" s="59" t="s">
         <v>15</v>
       </c>
       <c r="G16" s="59"/>
-      <c r="H16" s="7"/>
-      <c r="I16" s="16"/>
-      <c r="J16" s="7"/>
+      <c r="H16" s="7">
+        <f>SUM(B14:C14)</f>
+        <v>600</v>
+      </c>
+      <c r="I16" s="16" t="s">
+        <v>115</v>
+      </c>
+      <c r="J16" s="7">
+        <f>I5</f>
+        <v>400</v>
+      </c>
     </row>
-    <row r="17" spans="6:10" x14ac:dyDescent="0.2">
+    <row r="17" spans="6:10" x14ac:dyDescent="0.25">
       <c r="F17" s="59" t="s">
         <v>16</v>
       </c>
       <c r="G17" s="59"/>
-      <c r="H17" s="7"/>
-      <c r="I17" s="16"/>
-      <c r="J17" s="7"/>
+      <c r="H17" s="7">
+        <f>SUM(C13:C14)</f>
+        <v>520</v>
+      </c>
+      <c r="I17" s="16" t="s">
+        <v>115</v>
+      </c>
+      <c r="J17" s="7">
+        <f>SUM(B13:B14)</f>
+        <v>480</v>
+      </c>
     </row>
-    <row r="18" spans="6:10" x14ac:dyDescent="0.2">
+    <row r="18" spans="6:10" x14ac:dyDescent="0.25">
       <c r="F18" s="59" t="s">
         <v>17</v>
       </c>
       <c r="G18" s="59"/>
-      <c r="H18" s="7"/>
-      <c r="I18" s="16"/>
-      <c r="J18" s="7"/>
+      <c r="H18" s="7">
+        <f>C13</f>
+        <v>160</v>
+      </c>
+      <c r="I18" s="16" t="s">
+        <v>115</v>
+      </c>
+      <c r="J18" s="7">
+        <f>SUM(I6*SUM(B13:C13))</f>
+        <v>160</v>
+      </c>
     </row>
-    <row r="19" spans="6:10" x14ac:dyDescent="0.2">
+    <row r="19" spans="6:10" x14ac:dyDescent="0.25">
       <c r="F19" s="59" t="s">
         <v>18</v>
       </c>
       <c r="G19" s="59"/>
-      <c r="H19" s="7"/>
-      <c r="I19" s="16"/>
-      <c r="J19" s="7"/>
+      <c r="H19" s="7">
+        <f>C14</f>
+        <v>360</v>
+      </c>
+      <c r="I19" s="16" t="s">
+        <v>115</v>
+      </c>
+      <c r="J19" s="7">
+        <f>SUM(I7*SUM(B14:C14))</f>
+        <v>360</v>
+      </c>
     </row>
   </sheetData>
   <scenarios current="0" show="0">
@@ -17385,25 +17652,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:I29"/>
   <sheetViews>
-    <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="H34" sqref="H34"/>
+    <sheetView tabSelected="1" topLeftCell="A29" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.6640625" style="13" customWidth="1"/>
-    <col min="2" max="2" width="15.83203125" style="13" customWidth="1"/>
-    <col min="3" max="3" width="13.6640625" style="13" customWidth="1"/>
+    <col min="1" max="1" width="14.7109375" style="13" customWidth="1"/>
+    <col min="2" max="2" width="15.85546875" style="13" customWidth="1"/>
+    <col min="3" max="3" width="13.7109375" style="13" customWidth="1"/>
     <col min="4" max="4" width="13" style="13" customWidth="1"/>
-    <col min="5" max="5" width="8.83203125" style="13"/>
-    <col min="6" max="6" width="43.33203125" style="13" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.5" style="13" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="8.83203125" style="13"/>
-    <col min="9" max="9" width="12.5" style="13" bestFit="1" customWidth="1"/>
-    <col min="10" max="16384" width="8.83203125" style="13"/>
+    <col min="5" max="5" width="8.85546875" style="13"/>
+    <col min="6" max="6" width="43.28515625" style="13" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.42578125" style="13" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.85546875" style="13"/>
+    <col min="9" max="9" width="12.42578125" style="13" bestFit="1" customWidth="1"/>
+    <col min="10" max="16384" width="8.85546875" style="13"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="63" t="s">
         <v>109</v>
       </c>
@@ -17414,7 +17681,7 @@
       <c r="F1" s="63"/>
       <c r="G1" s="63"/>
     </row>
-    <row r="2" spans="1:9" ht="34" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:9" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A2" s="10" t="s">
         <v>27</v>
       </c>
@@ -17425,7 +17692,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="12" t="s">
         <v>28</v>
       </c>
@@ -17442,7 +17709,7 @@
         <v>282000</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="12" t="s">
         <v>3</v>
       </c>
@@ -17459,7 +17726,7 @@
         <v>50000</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="12" t="s">
         <v>29</v>
       </c>
@@ -17476,7 +17743,7 @@
         <v>75000</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="55" t="s">
         <v>21</v>
       </c>
@@ -17488,7 +17755,7 @@
       </c>
       <c r="G8" s="62"/>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B9" s="10" t="s">
         <v>24</v>
       </c>
@@ -17501,31 +17768,48 @@
       <c r="F9" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="G9" s="14"/>
+      <c r="G9" s="14">
+        <f>SUM(B3*SUM(B10:D10)+B4*SUM(B11:D11)+B5*D12)</f>
+        <v>199000</v>
+      </c>
     </row>
-    <row r="10" spans="1:9" ht="34" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:9" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A10" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="B10" s="14"/>
-      <c r="C10" s="14"/>
-      <c r="D10" s="14"/>
+      <c r="B10" s="14">
+        <v>4</v>
+      </c>
+      <c r="C10" s="14">
+        <v>4.9999999999999991</v>
+      </c>
+      <c r="D10" s="14">
+        <v>6</v>
+      </c>
     </row>
-    <row r="11" spans="1:9" ht="34" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:9" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A11" s="11" t="s">
         <v>104</v>
       </c>
-      <c r="B11" s="14"/>
-      <c r="C11" s="14"/>
-      <c r="D11" s="14"/>
+      <c r="B11" s="14">
+        <v>1.0000000000000002</v>
+      </c>
+      <c r="C11" s="14">
+        <v>0</v>
+      </c>
+      <c r="D11" s="14">
+        <v>0</v>
+      </c>
     </row>
-    <row r="12" spans="1:9" ht="51" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:9" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A12" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="D12" s="14"/>
+      <c r="D12" s="14">
+        <v>2</v>
+      </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="F13" s="55" t="s">
         <v>110</v>
       </c>
@@ -17533,133 +17817,248 @@
       <c r="H13" s="55"/>
       <c r="I13" s="55"/>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="F14" s="15" t="s">
         <v>33</v>
       </c>
-      <c r="G14" s="14"/>
-      <c r="H14" s="12"/>
-      <c r="I14" s="14"/>
+      <c r="G14" s="14">
+        <f>SUM(B10:D10)</f>
+        <v>15</v>
+      </c>
+      <c r="H14" s="12" t="s">
+        <v>115</v>
+      </c>
+      <c r="I14" s="14">
+        <v>1</v>
+      </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="F15" s="15" t="s">
         <v>34</v>
       </c>
-      <c r="G15" s="14"/>
-      <c r="H15" s="12"/>
-      <c r="I15" s="14"/>
+      <c r="G15" s="14">
+        <f>SUM(B11:D11)</f>
+        <v>1.0000000000000002</v>
+      </c>
+      <c r="H15" s="12" t="s">
+        <v>115</v>
+      </c>
+      <c r="I15" s="14">
+        <v>1</v>
+      </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="F16" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="G16" s="14"/>
-      <c r="H16" s="12"/>
-      <c r="I16" s="14"/>
+      <c r="G16" s="14">
+        <f>D12</f>
+        <v>2</v>
+      </c>
+      <c r="H16" s="12" t="s">
+        <v>115</v>
+      </c>
+      <c r="I16" s="14">
+        <v>1</v>
+      </c>
     </row>
-    <row r="17" spans="6:9" x14ac:dyDescent="0.2">
+    <row r="17" spans="6:9" x14ac:dyDescent="0.25">
       <c r="F17" s="15" t="s">
         <v>37</v>
       </c>
-      <c r="G17" s="14"/>
-      <c r="H17" s="12"/>
-      <c r="I17" s="14"/>
+      <c r="G17" s="14">
+        <f>B10</f>
+        <v>4</v>
+      </c>
+      <c r="H17" s="12" t="s">
+        <v>114</v>
+      </c>
+      <c r="I17" s="14">
+        <v>10</v>
+      </c>
     </row>
-    <row r="18" spans="6:9" x14ac:dyDescent="0.2">
+    <row r="18" spans="6:9" x14ac:dyDescent="0.25">
       <c r="F18" s="15" t="s">
         <v>36</v>
       </c>
-      <c r="G18" s="14"/>
-      <c r="H18" s="12"/>
-      <c r="I18" s="14"/>
+      <c r="G18" s="14">
+        <f>C10</f>
+        <v>4.9999999999999991</v>
+      </c>
+      <c r="H18" s="12" t="s">
+        <v>114</v>
+      </c>
+      <c r="I18" s="14">
+        <v>10</v>
+      </c>
     </row>
-    <row r="19" spans="6:9" x14ac:dyDescent="0.2">
+    <row r="19" spans="6:9" x14ac:dyDescent="0.25">
       <c r="F19" s="15" t="s">
         <v>38</v>
       </c>
-      <c r="G19" s="14"/>
-      <c r="H19" s="12"/>
-      <c r="I19" s="14"/>
+      <c r="G19" s="14">
+        <f>D10</f>
+        <v>6</v>
+      </c>
+      <c r="H19" s="12" t="s">
+        <v>114</v>
+      </c>
+      <c r="I19" s="14">
+        <v>10</v>
+      </c>
     </row>
-    <row r="20" spans="6:9" x14ac:dyDescent="0.2">
+    <row r="20" spans="6:9" x14ac:dyDescent="0.25">
       <c r="F20" s="15" t="s">
         <v>39</v>
       </c>
-      <c r="G20" s="14"/>
-      <c r="H20" s="12"/>
-      <c r="I20" s="14"/>
+      <c r="G20" s="14">
+        <f>B11</f>
+        <v>1.0000000000000002</v>
+      </c>
+      <c r="H20" s="12" t="s">
+        <v>114</v>
+      </c>
+      <c r="I20" s="14">
+        <v>6</v>
+      </c>
     </row>
-    <row r="21" spans="6:9" x14ac:dyDescent="0.2">
+    <row r="21" spans="6:9" x14ac:dyDescent="0.25">
       <c r="F21" s="15" t="s">
         <v>40</v>
       </c>
-      <c r="G21" s="14"/>
-      <c r="H21" s="12"/>
-      <c r="I21" s="14"/>
+      <c r="G21" s="14">
+        <f>C11</f>
+        <v>0</v>
+      </c>
+      <c r="H21" s="12" t="s">
+        <v>114</v>
+      </c>
+      <c r="I21" s="14">
+        <v>6</v>
+      </c>
     </row>
-    <row r="22" spans="6:9" x14ac:dyDescent="0.2">
+    <row r="22" spans="6:9" x14ac:dyDescent="0.25">
       <c r="F22" s="15" t="s">
         <v>41</v>
       </c>
-      <c r="G22" s="14"/>
-      <c r="H22" s="12"/>
-      <c r="I22" s="14"/>
+      <c r="G22" s="14">
+        <f>D11</f>
+        <v>0</v>
+      </c>
+      <c r="H22" s="12" t="s">
+        <v>114</v>
+      </c>
+      <c r="I22" s="14">
+        <v>6</v>
+      </c>
     </row>
-    <row r="23" spans="6:9" x14ac:dyDescent="0.2">
+    <row r="23" spans="6:9" x14ac:dyDescent="0.25">
       <c r="F23" s="15" t="s">
         <v>48</v>
       </c>
-      <c r="G23" s="14"/>
-      <c r="H23" s="12"/>
-      <c r="I23" s="14"/>
+      <c r="G23" s="14">
+        <f>D12</f>
+        <v>2</v>
+      </c>
+      <c r="H23" s="12" t="s">
+        <v>114</v>
+      </c>
+      <c r="I23" s="14">
+        <v>2</v>
+      </c>
     </row>
-    <row r="24" spans="6:9" x14ac:dyDescent="0.2">
+    <row r="24" spans="6:9" x14ac:dyDescent="0.25">
       <c r="F24" s="15" t="s">
         <v>42</v>
       </c>
-      <c r="G24" s="14"/>
-      <c r="H24" s="12"/>
-      <c r="I24" s="14"/>
+      <c r="G24" s="14">
+        <f>SUM(B10:B11)</f>
+        <v>5</v>
+      </c>
+      <c r="H24" s="12" t="s">
+        <v>115</v>
+      </c>
+      <c r="I24" s="14">
+        <v>5</v>
+      </c>
     </row>
-    <row r="25" spans="6:9" x14ac:dyDescent="0.2">
+    <row r="25" spans="6:9" x14ac:dyDescent="0.25">
       <c r="F25" s="15" t="s">
         <v>43</v>
       </c>
-      <c r="G25" s="14"/>
-      <c r="H25" s="12"/>
-      <c r="I25" s="14"/>
+      <c r="G25" s="14">
+        <f>SUM(C10:C11)</f>
+        <v>4.9999999999999991</v>
+      </c>
+      <c r="H25" s="12" t="s">
+        <v>115</v>
+      </c>
+      <c r="I25" s="14">
+        <v>5</v>
+      </c>
     </row>
-    <row r="26" spans="6:9" x14ac:dyDescent="0.2">
+    <row r="26" spans="6:9" x14ac:dyDescent="0.25">
       <c r="F26" s="15" t="s">
         <v>44</v>
       </c>
-      <c r="G26" s="14"/>
-      <c r="H26" s="12"/>
-      <c r="I26" s="14"/>
+      <c r="G26" s="14">
+        <f>SUM(D10:D12)</f>
+        <v>8</v>
+      </c>
+      <c r="H26" s="12" t="s">
+        <v>115</v>
+      </c>
+      <c r="I26" s="14">
+        <v>5</v>
+      </c>
     </row>
-    <row r="27" spans="6:9" x14ac:dyDescent="0.2">
+    <row r="27" spans="6:9" x14ac:dyDescent="0.25">
       <c r="F27" s="15" t="s">
         <v>45</v>
       </c>
-      <c r="G27" s="27"/>
-      <c r="H27" s="12"/>
-      <c r="I27" s="27"/>
+      <c r="G27" s="27">
+        <f>SUM(C3*B10+C4*B11)</f>
+        <v>27000</v>
+      </c>
+      <c r="H27" s="12" t="s">
+        <v>114</v>
+      </c>
+      <c r="I27" s="27">
+        <f>G4</f>
+        <v>50000</v>
+      </c>
     </row>
-    <row r="28" spans="6:9" x14ac:dyDescent="0.2">
+    <row r="28" spans="6:9" x14ac:dyDescent="0.25">
       <c r="F28" s="15" t="s">
         <v>46</v>
       </c>
-      <c r="G28" s="27"/>
-      <c r="H28" s="12"/>
-      <c r="I28" s="27"/>
+      <c r="G28" s="27">
+        <f>SUM(C3*C10+C4*C11)</f>
+        <v>24999.999999999996</v>
+      </c>
+      <c r="H28" s="12" t="s">
+        <v>114</v>
+      </c>
+      <c r="I28" s="27">
+        <f>G5</f>
+        <v>75000</v>
+      </c>
     </row>
-    <row r="29" spans="6:9" x14ac:dyDescent="0.2">
+    <row r="29" spans="6:9" x14ac:dyDescent="0.25">
       <c r="F29" s="15" t="s">
         <v>47</v>
       </c>
-      <c r="G29" s="27"/>
-      <c r="H29" s="12"/>
-      <c r="I29" s="27"/>
+      <c r="G29" s="27">
+        <f>SUM(C3*SUM(B10:D10)+C4*SUM(B11:D11)+C5*D12)</f>
+        <v>282000</v>
+      </c>
+      <c r="H29" s="12" t="s">
+        <v>114</v>
+      </c>
+      <c r="I29" s="27">
+        <f>G3</f>
+        <v>282000</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="4">

</xml_diff>